<commit_message>
added guest checkout support
Signed-off-by: Ibrahem Batta <18301319+ibatta@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet _back.xlsx
+++ b/src/com/generic/config/DataSheet _back.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14175" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="20790" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="176">
   <si>
     <t>aa@gg.cc</t>
   </si>
@@ -473,6 +473,100 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+  <si>
+    <t>2223</t>
+  </si>
+  <si>
+    <t>2224</t>
+  </si>
+  <si>
+    <t>2225</t>
+  </si>
+  <si>
+    <t>2226</t>
+  </si>
+  <si>
+    <t>£10.99</t>
+  </si>
+  <si>
+    <t>£53.36</t>
+  </si>
+  <si>
+    <t>Your order includes £8.89 tax.</t>
+  </si>
+  <si>
+    <t>£64.35</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001269</t>
+  </si>
+  <si>
+    <t>£77.16</t>
+  </si>
+  <si>
+    <t>Your order includes £12.86 tax.</t>
+  </si>
+  <si>
+    <t>£88.15</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001271</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>fresh
+new-user
+new-shipping
+new-payment</t>
+  </si>
+  <si>
+    <t>£38.58</t>
+  </si>
+  <si>
+    <t>Your order includes £6.43 tax.</t>
+  </si>
+  <si>
+    <t>£49.57</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001279</t>
+  </si>
+  <si>
+    <t>etqpo5826@random.com</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>guest
+new-user
+new-shipping
+new-payment</t>
+  </si>
+  <si>
+    <t>guest user with new visa payment and shipping address</t>
+  </si>
+  <si>
+    <t>fresh user with new visa payment and shipping address</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001296</t>
+  </si>
+  <si>
+    <t>£5.99</t>
+  </si>
+  <si>
+    <t>£44.57</t>
   </si>
 </sst>
 </file>
@@ -616,7 +710,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -706,6 +800,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1345,9 +1448,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1359,11 +1464,11 @@
     <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1395,7 +1500,7 @@
       <c r="I1" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="32" t="s">
         <v>108</v>
       </c>
       <c r="K1" s="18" t="s">
@@ -1421,9 +1526,7 @@
       <c r="A2" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>105</v>
-      </c>
+      <c r="B2" s="29"/>
       <c r="C2" s="10" t="s">
         <v>60</v>
       </c>
@@ -1445,23 +1548,24 @@
       <c r="I2" s="13" t="s">
         <v>87</v>
       </c>
+      <c r="J2" s="5"/>
       <c r="K2" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="13" t="s">
-        <v>147</v>
+      <c r="L2" s="34" t="s">
+        <v>157</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>147</v>
+        <v>158</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="6" customFormat="1" ht="60">
@@ -1490,15 +1594,25 @@
       <c r="I3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="13"/>
+      <c r="J3" s="33"/>
       <c r="K3" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="15"/>
+      <c r="L3" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="4" spans="1:16" ht="60">
       <c r="A4" s="29" t="s">
@@ -1526,23 +1640,31 @@
       <c r="I4" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="J4" s="13"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="15"/>
+      <c r="L4" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="5" spans="1:16" ht="60">
       <c r="A5" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>105</v>
-      </c>
+      <c r="B5" s="29"/>
       <c r="C5" s="10" t="s">
         <v>62</v>
       </c>
@@ -1570,20 +1692,20 @@
       <c r="K5" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>147</v>
+      <c r="L5" s="34" t="s">
+        <v>161</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>147</v>
+        <v>154</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="60">
@@ -1616,11 +1738,21 @@
       <c r="K6" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="15"/>
+      <c r="L6" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="7" spans="1:16" ht="60">
       <c r="A7" s="29" t="s">
@@ -1654,11 +1786,21 @@
       <c r="K7" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="15"/>
+      <c r="L7" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="8" spans="1:16" ht="60">
       <c r="A8" s="29" t="s">
@@ -1690,11 +1832,21 @@
       <c r="K8" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="15"/>
+      <c r="L8" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="60">
       <c r="A9" s="29" t="s">
@@ -1702,19 +1854,19 @@
       </c>
       <c r="B9" s="29"/>
       <c r="C9" s="10" t="s">
-        <v>63</v>
+        <v>172</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>86</v>
@@ -1722,20 +1874,122 @@
       <c r="I9" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="J9" s="13"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="L9" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="60">
+      <c r="A10" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="15"/>
+      <c r="L10" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="60">
+      <c r="A11" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>174</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K9" r:id="rId2"/>
+    <hyperlink ref="K10" r:id="rId2"/>
     <hyperlink ref="K3" r:id="rId3"/>
     <hyperlink ref="K8" r:id="rId4"/>
     <hyperlink ref="K4:K7" r:id="rId5" display="ibatta@dbi.com"/>

</xml_diff>

<commit_message>
finished checkout test template
Signed-off-by: Ibrahem Batta <18301319+ibatta@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet _back.xlsx
+++ b/src/com/generic/config/DataSheet _back.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="20790" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="25515" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="184">
   <si>
     <t>aa@gg.cc</t>
   </si>
@@ -433,9 +433,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -500,19 +497,6 @@
   </si>
   <si>
     <t>£64.35</t>
-  </si>
-  <si>
-    <t>ORDER NUMBER
-00001269</t>
-  </si>
-  <si>
-    <t>£77.16</t>
-  </si>
-  <si>
-    <t>Your order includes £12.86 tax.</t>
-  </si>
-  <si>
-    <t>£88.15</t>
   </si>
   <si>
     <t>ORDER NUMBER
@@ -537,13 +521,6 @@
     <t>£49.57</t>
   </si>
   <si>
-    <t>ORDER NUMBER
-00001279</t>
-  </si>
-  <si>
-    <t>etqpo5826@random.com</t>
-  </si>
-  <si>
     <t>T10</t>
   </si>
   <si>
@@ -559,14 +536,67 @@
     <t>fresh user with new visa payment and shipping address</t>
   </si>
   <si>
+    <t>guest
+new-user
+new-shipping
+new-payment
+register-guest</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>£5.99</t>
+  </si>
+  <si>
+    <t>£44.57</t>
+  </si>
+  <si>
     <t>ORDER NUMBER
-00001296</t>
-  </si>
-  <si>
-    <t>£5.99</t>
-  </si>
-  <si>
-    <t>£44.57</t>
+00001309</t>
+  </si>
+  <si>
+    <t>£265.89</t>
+  </si>
+  <si>
+    <t>Your order includes £44.31 tax.</t>
+  </si>
+  <si>
+    <t>£276.88</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001311</t>
+  </si>
+  <si>
+    <t>abcdd5688@random.com</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001313</t>
+  </si>
+  <si>
+    <t>rtkgh630@random.com</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001315</t>
+  </si>
+  <si>
+    <t>sanlct6020@random.com</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER
+00001323</t>
+  </si>
+  <si>
+    <t>takqima2212@random.com</t>
+  </si>
+  <si>
+    <t>userName</t>
   </si>
 </sst>
 </file>
@@ -1448,10 +1478,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1464,7 +1494,7 @@
     <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1474,7 +1504,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="9" customFormat="1">
       <c r="A1" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>106</v>
@@ -1524,7 +1554,7 @@
     </row>
     <row r="2" spans="1:16" s="6" customFormat="1" ht="60">
       <c r="A2" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="10" t="s">
@@ -1553,24 +1583,24 @@
         <v>96</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="6" customFormat="1" ht="60">
       <c r="A3" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="10" t="s">
@@ -1599,16 +1629,16 @@
         <v>96</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="P3" s="14" t="s">
         <v>152</v>
@@ -1616,7 +1646,7 @@
     </row>
     <row r="4" spans="1:16" ht="60">
       <c r="A4" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="10" t="s">
@@ -1645,24 +1675,24 @@
         <v>96</v>
       </c>
       <c r="L4" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M4" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="N4" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="O4" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="P4" s="14" t="s">
         <v>151</v>
-      </c>
-      <c r="P4" s="14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="60">
       <c r="A5" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="10" t="s">
@@ -1693,24 +1723,24 @@
         <v>96</v>
       </c>
       <c r="L5" s="34" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N5" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="O5" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="O5" s="14" t="s">
-        <v>155</v>
-      </c>
       <c r="P5" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="60">
       <c r="A6" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="10" t="s">
@@ -1739,24 +1769,24 @@
         <v>96</v>
       </c>
       <c r="L6" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M6" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="N6" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="O6" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="P6" s="14" t="s">
         <v>151</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="60">
       <c r="A7" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="10" t="s">
@@ -1787,24 +1817,24 @@
         <v>96</v>
       </c>
       <c r="L7" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M7" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="N7" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="O7" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="O7" s="14" t="s">
+      <c r="P7" s="14" t="s">
         <v>151</v>
-      </c>
-      <c r="P7" s="14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="60">
       <c r="A8" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="10" t="s">
@@ -1833,31 +1863,33 @@
         <v>96</v>
       </c>
       <c r="L8" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M8" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="N8" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="O8" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="P8" s="14" t="s">
         <v>151</v>
-      </c>
-      <c r="P8" s="14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="60">
       <c r="A9" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="29"/>
+        <v>145</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>105</v>
+      </c>
       <c r="C9" s="10" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>120</v>
@@ -1876,27 +1908,27 @@
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="10" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="60">
       <c r="A10" s="29" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="10" t="s">
@@ -1925,33 +1957,31 @@
         <v>96</v>
       </c>
       <c r="L10" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M10" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="N10" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="O10" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="O10" s="14" t="s">
+      <c r="P10" s="14" t="s">
         <v>151</v>
-      </c>
-      <c r="P10" s="14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="60">
       <c r="A11" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>105</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="B11" s="29"/>
       <c r="C11" s="10" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>120</v>
@@ -1969,21 +1999,69 @@
         <v>87</v>
       </c>
       <c r="J11" s="13"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="10" t="s">
+        <v>177</v>
+      </c>
       <c r="L11" s="14" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="N11" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="75">
+      <c r="A12" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="O11" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="P11" s="14" t="s">
-        <v>174</v>
+      <c r="D12" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2004,51 +2082,72 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="21" t="s">
         <v>133</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" s="21">
-        <v>1234567</v>
-      </c>
-      <c r="D2" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="31" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2434,10 +2533,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection sqref="A1:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2460,7 +2559,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="9" customFormat="1">
       <c r="A1" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>106</v>
@@ -2486,7 +2585,7 @@
       <c r="I1" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="32" t="s">
         <v>108</v>
       </c>
       <c r="K1" s="18" t="s">
@@ -2510,7 +2609,7 @@
     </row>
     <row r="2" spans="1:16" s="6" customFormat="1" ht="60">
       <c r="A2" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>105</v>
@@ -2536,30 +2635,33 @@
       <c r="I2" s="13" t="s">
         <v>87</v>
       </c>
+      <c r="J2" s="5"/>
       <c r="K2" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L2" s="13" t="s">
-        <v>147</v>
+      <c r="L2" s="34" t="s">
+        <v>146</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="6" customFormat="1" ht="60">
       <c r="A3" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="29"/>
+        <v>139</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>105</v>
+      </c>
       <c r="C3" s="10" t="s">
         <v>60</v>
       </c>
@@ -2581,19 +2683,29 @@
       <c r="I3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="13"/>
+      <c r="J3" s="33"/>
       <c r="K3" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="15"/>
+      <c r="L3" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="4" spans="1:16" ht="60">
       <c r="A4" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="10" t="s">
@@ -2617,23 +2729,31 @@
       <c r="I4" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="J4" s="13"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="15"/>
-    </row>
-    <row r="5" spans="1:16" ht="60">
+      <c r="L4" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="75">
       <c r="A5" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>105</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B5" s="29"/>
       <c r="C5" s="10" t="s">
         <v>62</v>
       </c>
@@ -2661,25 +2781,25 @@
       <c r="K5" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L5" s="13" t="s">
-        <v>147</v>
+      <c r="L5" s="34" t="s">
+        <v>156</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>147</v>
+        <v>153</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="60">
       <c r="A6" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="10" t="s">
@@ -2707,15 +2827,25 @@
       <c r="K6" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="15"/>
+      <c r="L6" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="7" spans="1:16" ht="60">
       <c r="A7" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="10" t="s">
@@ -2745,15 +2875,25 @@
       <c r="K7" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="15"/>
+      <c r="L7" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="8" spans="1:16" ht="60">
       <c r="A8" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="10" t="s">
@@ -2781,31 +2921,43 @@
       <c r="K8" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="15"/>
-    </row>
-    <row r="9" spans="1:16" ht="60">
+      <c r="L8" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="75">
       <c r="A9" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="29"/>
+        <v>145</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>105</v>
+      </c>
       <c r="C9" s="10" t="s">
-        <v>63</v>
+        <v>165</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>86</v>
@@ -2813,20 +2965,172 @@
       <c r="I9" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="J9" s="13"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="L9" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="60">
+      <c r="A10" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="15"/>
+      <c r="L10" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="60">
+      <c r="A11" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="75">
+      <c r="A12" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>168</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K9" r:id="rId2"/>
+    <hyperlink ref="K10" r:id="rId2"/>
     <hyperlink ref="K3" r:id="rId3"/>
     <hyperlink ref="K8" r:id="rId4"/>
     <hyperlink ref="K4:K7" r:id="rId5" display="ibatta@dbi.com"/>

</xml_diff>

<commit_message>
quick view mail sign up
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet _back.xlsx
+++ b/src/com/generic/config/DataSheet _back.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="182985" yWindow="0" windowWidth="16980" windowHeight="7020"/>
+    <workbookView xWindow="185775" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3583" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3581" uniqueCount="948">
   <si>
     <t>Please enter a valid email</t>
   </si>
@@ -1860,9 +1860,6 @@
   </si>
   <si>
     <t>PLP with lowest price first</t>
-  </si>
-  <si>
-    <t>https://hybrisdemo.conexus.co.uk:9002/yacceleratorstorefront/en/Brands/667/c/667</t>
   </si>
   <si>
     <t>Top Rated</t>
@@ -2944,6 +2941,18 @@
     <t>P1
 P2
 P4</t>
+  </si>
+  <si>
+    <t>PLP1</t>
+  </si>
+  <si>
+    <t>PLP2</t>
+  </si>
+  <si>
+    <t>PLP3</t>
+  </si>
+  <si>
+    <t>PLP4</t>
   </si>
 </sst>
 </file>
@@ -3756,7 +3765,7 @@
   </sheetPr>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
@@ -3798,7 +3807,7 @@
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1">
       <c r="A2" s="20" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>66</v>
@@ -3819,12 +3828,12 @@
         <v>47</v>
       </c>
       <c r="H2" s="90" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1">
       <c r="A3" s="20" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="24" t="s">
@@ -3843,12 +3852,12 @@
         <v>48</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1">
       <c r="A4" s="20" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="24" t="s">
@@ -3867,12 +3876,12 @@
         <v>47</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1">
       <c r="A5" s="20" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>66</v>
@@ -3893,12 +3902,12 @@
         <v>47</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1">
       <c r="A6" s="20" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>66</v>
@@ -3919,12 +3928,12 @@
         <v>48</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1">
       <c r="A7" s="20" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>66</v>
@@ -3945,12 +3954,12 @@
         <v>47</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="20" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="24" t="s">
@@ -3969,12 +3978,12 @@
         <v>47</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="20" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="24" t="s">
@@ -3993,12 +4002,12 @@
         <v>48</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="20" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="24" t="s">
@@ -4017,12 +4026,12 @@
         <v>47</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="20" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="24" t="s">
@@ -4041,12 +4050,12 @@
         <v>47</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="20" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="24" t="s">
@@ -4065,12 +4074,12 @@
         <v>48</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="20" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="24" t="s">
@@ -4089,12 +4098,12 @@
         <v>47</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="20" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="24" t="s">
@@ -4113,12 +4122,12 @@
         <v>47</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="20" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="24" t="s">
@@ -4137,12 +4146,12 @@
         <v>48</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="20" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="24" t="s">
@@ -4161,12 +4170,12 @@
         <v>47</v>
       </c>
       <c r="H16" s="40" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="20" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>66</v>
@@ -4187,12 +4196,12 @@
         <v>47</v>
       </c>
       <c r="H17" s="40" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="20" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="24" t="s">
@@ -4211,12 +4220,12 @@
         <v>48</v>
       </c>
       <c r="H18" s="40" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="20" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="24" t="s">
@@ -4235,12 +4244,12 @@
         <v>47</v>
       </c>
       <c r="H19" s="40" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="20" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="24" t="s">
@@ -4259,12 +4268,12 @@
         <v>47</v>
       </c>
       <c r="H20" s="40" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="20" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="24" t="s">
@@ -4283,12 +4292,12 @@
         <v>48</v>
       </c>
       <c r="H21" s="40" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="20" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="24" t="s">
@@ -4307,12 +4316,12 @@
         <v>47</v>
       </c>
       <c r="H22" s="40" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="20" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>66</v>
@@ -4333,12 +4342,12 @@
         <v>47</v>
       </c>
       <c r="H23" s="40" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="20" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>66</v>
@@ -4359,12 +4368,12 @@
         <v>48</v>
       </c>
       <c r="H24" s="40" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="20" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>66</v>
@@ -4385,12 +4394,12 @@
         <v>47</v>
       </c>
       <c r="H25" s="40" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="20" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>66</v>
@@ -4411,12 +4420,12 @@
         <v>47</v>
       </c>
       <c r="H26" s="40" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="20" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="24" t="s">
@@ -4435,12 +4444,12 @@
         <v>48</v>
       </c>
       <c r="H27" s="40" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="20" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="24" t="s">
@@ -4459,12 +4468,12 @@
         <v>47</v>
       </c>
       <c r="H28" s="40" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="20" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B29" s="20"/>
       <c r="C29" s="24" t="s">
@@ -4483,12 +4492,12 @@
         <v>47</v>
       </c>
       <c r="H29" s="40" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="20" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B30" s="20"/>
       <c r="C30" s="24" t="s">
@@ -4507,12 +4516,12 @@
         <v>48</v>
       </c>
       <c r="H30" s="40" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="20" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="24" t="s">
@@ -4531,12 +4540,12 @@
         <v>47</v>
       </c>
       <c r="H31" s="40" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="20" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B32" s="20"/>
       <c r="C32" s="24" t="s">
@@ -4555,12 +4564,12 @@
         <v>47</v>
       </c>
       <c r="H32" s="40" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="20" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B33" s="20" t="s">
         <v>66</v>
@@ -4581,12 +4590,12 @@
         <v>48</v>
       </c>
       <c r="H33" s="40" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="20" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="24" t="s">
@@ -4605,12 +4614,12 @@
         <v>47</v>
       </c>
       <c r="H34" s="40" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="20" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="24" t="s">
@@ -4629,12 +4638,12 @@
         <v>47</v>
       </c>
       <c r="H35" s="40" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="20" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="24" t="s">
@@ -4653,12 +4662,12 @@
         <v>48</v>
       </c>
       <c r="H36" s="40" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="20" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="24" t="s">
@@ -4677,12 +4686,12 @@
         <v>47</v>
       </c>
       <c r="H37" s="40" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="20" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="24" t="s">
@@ -4701,7 +4710,7 @@
         <v>47</v>
       </c>
       <c r="H38" s="40" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
   </sheetData>
@@ -4770,10 +4779,10 @@
         <v>66</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>170</v>
@@ -4788,7 +4797,7 @@
         <v>47</v>
       </c>
       <c r="I2" s="58" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>257</v>
@@ -4802,10 +4811,10 @@
         <v>66</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E3" s="28" t="s">
         <v>170</v>
@@ -4820,7 +4829,7 @@
         <v>47</v>
       </c>
       <c r="I3" s="58" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J3" s="39" t="s">
         <v>256</v>
@@ -4864,7 +4873,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4875,11 +4884,11 @@
         <v>66</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="64" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4890,11 +4899,11 @@
         <v>66</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4905,10 +4914,10 @@
         <v>66</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E4" s="14"/>
     </row>
@@ -4961,39 +4970,39 @@
         <v>16</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>663</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>664</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>665</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>90</v>
       </c>
       <c r="I1" s="78" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>665</v>
+      </c>
+      <c r="K1" s="67" t="s">
         <v>666</v>
       </c>
-      <c r="K1" s="67" t="s">
+      <c r="L1" s="67" t="s">
         <v>667</v>
-      </c>
-      <c r="L1" s="67" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="46" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E2" s="89" t="s">
         <v>268</v>
@@ -5008,23 +5017,23 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="46" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B3" s="46"/>
       <c r="C3" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E3" s="66" t="s">
         <v>258</v>
       </c>
       <c r="F3" s="66" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G3" s="66" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="H3" s="2">
         <v>1234567</v>
@@ -5036,29 +5045,29 @@
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="46" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B4" s="46"/>
       <c r="C4" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E4" s="89" t="s">
         <v>259</v>
       </c>
       <c r="F4" s="89" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G4" s="89" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="H4" s="2">
         <v>1234567</v>
       </c>
       <c r="I4" s="88" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
@@ -5066,27 +5075,27 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="46" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B5" s="46"/>
       <c r="C5" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>260</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="39" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H5" s="2">
         <v>1234567</v>
       </c>
       <c r="I5" s="88" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J5" s="88" t="s">
         <v>0</v>
@@ -5096,89 +5105,89 @@
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" s="46" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B6" s="46"/>
       <c r="C6" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E6" s="39" t="s">
         <v>261</v>
       </c>
       <c r="F6" s="89" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G6" s="28"/>
       <c r="H6" s="2">
         <v>1234567</v>
       </c>
       <c r="I6" s="88" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J6" s="88"/>
       <c r="K6" s="88" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L6" s="63"/>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" s="46" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B7" s="46"/>
       <c r="C7" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E7" s="39" t="s">
         <v>262</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="88" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J7" s="88"/>
       <c r="K7" s="88"/>
       <c r="L7" s="63" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="46" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B8" s="46"/>
       <c r="C8" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>263</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H8" s="2">
         <v>1234567</v>
       </c>
       <c r="I8" s="88" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J8" t="s">
         <v>0</v>
@@ -5188,128 +5197,128 @@
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="46" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B9" s="46"/>
       <c r="C9" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E9" s="39" t="s">
         <v>264</v>
       </c>
       <c r="F9" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H9" s="2">
         <v>1234567</v>
       </c>
       <c r="I9" s="88" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J9" s="88"/>
       <c r="K9" s="88" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="L9" s="63"/>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" s="46" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B10" s="46"/>
       <c r="C10" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E10" s="39" t="s">
         <v>265</v>
       </c>
       <c r="F10" s="39" t="s">
+        <v>861</v>
+      </c>
+      <c r="G10" s="39" t="s">
         <v>862</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>863</v>
       </c>
       <c r="H10" s="2">
         <v>1234567</v>
       </c>
       <c r="I10" s="88" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J10" s="88"/>
       <c r="K10" s="88" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="L10" s="63"/>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="46" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B11" s="46"/>
       <c r="C11" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E11" s="39" t="s">
         <v>266</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="H11" s="2">
         <v>874531324</v>
       </c>
       <c r="I11" s="88" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J11" s="88"/>
       <c r="K11" s="88"/>
       <c r="L11" s="63" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="46" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B12" s="46"/>
       <c r="C12" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>687</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>688</v>
       </c>
       <c r="E12" s="39" t="s">
         <v>267</v>
       </c>
       <c r="F12" s="39" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G12" s="39" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H12" s="2">
         <v>1234567</v>
       </c>
       <c r="I12" s="88" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J12" s="88" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="K12" s="88"/>
       <c r="L12" s="63"/>
@@ -5361,7 +5370,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>574</v>
@@ -5417,19 +5426,19 @@
         <v>66</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>592</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>593</v>
       </c>
       <c r="H2" s="47">
         <v>300389093</v>
@@ -5444,7 +5453,7 @@
         <v>3</v>
       </c>
       <c r="L2" s="49" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="M2" s="50">
         <v>3</v>
@@ -5476,19 +5485,19 @@
         <v>66</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>596</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>597</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>598</v>
       </c>
       <c r="H3" s="47">
         <v>300389094</v>
@@ -5503,7 +5512,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="M3" s="50">
         <v>2</v>
@@ -5535,19 +5544,19 @@
         <v>66</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="H4" s="47">
         <v>300389095</v>
@@ -5562,7 +5571,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="M4" s="50">
         <v>1</v>
@@ -5594,19 +5603,19 @@
         <v>66</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="H5" s="47">
         <v>300389095</v>
@@ -5653,10 +5662,10 @@
         <v>66</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -5729,7 +5738,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="67" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30">
@@ -5740,13 +5749,13 @@
         <v>66</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E2" s="63" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5757,10 +5766,10 @@
         <v>66</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E3" s="63">
         <v>500</v>
@@ -5780,16 +5789,21 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="10" max="11" width="37.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="32.85546875" customWidth="1"/>
+    <col min="11" max="11" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>93</v>
       </c>
@@ -5818,13 +5832,13 @@
         <v>50</v>
       </c>
       <c r="J1" s="78" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="K1" s="38" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="90">
+    <row r="2" spans="1:11" ht="60">
       <c r="A2" s="56" t="s">
         <v>94</v>
       </c>
@@ -5832,10 +5846,10 @@
         <v>66</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D2" s="76" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E2" s="77" t="s">
         <v>5</v>
@@ -5853,13 +5867,13 @@
         <v>47</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="90">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60">
       <c r="A3" s="56" t="s">
         <v>95</v>
       </c>
@@ -5867,10 +5881,10 @@
         <v>66</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D3" s="76" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E3" s="77" t="s">
         <v>5</v>
@@ -5888,13 +5902,13 @@
         <v>47</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="K3" s="66" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="105">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60">
       <c r="A4" s="56" t="s">
         <v>96</v>
       </c>
@@ -5902,10 +5916,10 @@
         <v>66</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D4" s="76" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E4" s="77" t="s">
         <v>5</v>
@@ -5923,13 +5937,13 @@
         <v>47</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="K4" s="66" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="90">
+    <row r="5" spans="1:11" ht="60">
       <c r="A5" s="56" t="s">
         <v>97</v>
       </c>
@@ -5937,10 +5951,10 @@
         <v>66</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D5" s="76" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E5" s="77" t="s">
         <v>5</v>
@@ -5958,13 +5972,13 @@
         <v>47</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="K5" s="66" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="90">
+    <row r="6" spans="1:11" ht="60">
       <c r="A6" s="56" t="s">
         <v>98</v>
       </c>
@@ -5972,10 +5986,10 @@
         <v>66</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D6" s="76" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E6" s="77" t="s">
         <v>5</v>
@@ -5993,13 +6007,13 @@
         <v>47</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="K6" s="28" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="90">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="60">
       <c r="A7" s="56" t="s">
         <v>99</v>
       </c>
@@ -6007,10 +6021,10 @@
         <v>66</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D7" s="76" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E7" s="77" t="s">
         <v>5</v>
@@ -6028,10 +6042,10 @@
         <v>47</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="K7" s="28" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60">
@@ -6042,10 +6056,10 @@
         <v>66</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D8" s="76" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E8" s="77" t="s">
         <v>5</v>
@@ -6063,13 +6077,13 @@
         <v>47</v>
       </c>
       <c r="J8" s="28" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="K8" s="28" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="90">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45">
       <c r="A9" s="56" t="s">
         <v>101</v>
       </c>
@@ -6077,10 +6091,10 @@
         <v>66</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E9" s="77" t="s">
         <v>5</v>
@@ -6092,19 +6106,19 @@
         <v>19</v>
       </c>
       <c r="H9" s="76" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I9" s="76" t="s">
         <v>47</v>
       </c>
       <c r="J9" s="28" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="K9" s="28" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="90">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45">
       <c r="A10" s="56" t="s">
         <v>103</v>
       </c>
@@ -6112,10 +6126,10 @@
         <v>66</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E10" s="77" t="s">
         <v>5</v>
@@ -6127,19 +6141,19 @@
         <v>19</v>
       </c>
       <c r="H10" s="76" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I10" s="76" t="s">
         <v>47</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="K10" s="28" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="90">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45">
       <c r="A11" s="56" t="s">
         <v>104</v>
       </c>
@@ -6147,10 +6161,10 @@
         <v>66</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E11" s="77" t="s">
         <v>5</v>
@@ -6162,19 +6176,19 @@
         <v>19</v>
       </c>
       <c r="H11" s="76" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I11" s="76" t="s">
         <v>47</v>
       </c>
       <c r="J11" s="28" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="K11" s="28" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="90">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="45">
       <c r="A12" s="56" t="s">
         <v>106</v>
       </c>
@@ -6182,10 +6196,10 @@
         <v>66</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E12" s="77" t="s">
         <v>5</v>
@@ -6197,19 +6211,19 @@
         <v>19</v>
       </c>
       <c r="H12" s="76" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I12" s="76" t="s">
         <v>47</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="K12" s="28" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="90">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="45">
       <c r="A13" s="56" t="s">
         <v>129</v>
       </c>
@@ -6217,10 +6231,10 @@
         <v>66</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E13" s="77" t="s">
         <v>5</v>
@@ -6232,19 +6246,19 @@
         <v>19</v>
       </c>
       <c r="H13" s="76" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I13" s="76" t="s">
         <v>47</v>
       </c>
       <c r="J13" s="28" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="K13" s="28" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="90">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="45">
       <c r="A14" s="56" t="s">
         <v>130</v>
       </c>
@@ -6252,10 +6266,10 @@
         <v>66</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E14" s="77" t="s">
         <v>5</v>
@@ -6267,19 +6281,19 @@
         <v>19</v>
       </c>
       <c r="H14" s="76" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I14" s="76" t="s">
         <v>47</v>
       </c>
       <c r="J14" s="28" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="K14" s="28" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="90">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="45">
       <c r="A15" s="56" t="s">
         <v>131</v>
       </c>
@@ -6287,10 +6301,10 @@
         <v>66</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E15" s="77" t="s">
         <v>5</v>
@@ -6302,16 +6316,16 @@
         <v>19</v>
       </c>
       <c r="H15" s="76" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I15" s="76" t="s">
         <v>47</v>
       </c>
       <c r="J15" s="28" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="K15" s="28" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
   </sheetData>
@@ -6413,7 +6427,7 @@
         <v>70</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>15</v>
@@ -6429,7 +6443,7 @@
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L2" s="15" t="s">
         <v>102</v>
@@ -6459,7 +6473,7 @@
         <v>70</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>15</v>
@@ -6475,7 +6489,7 @@
       </c>
       <c r="J3" s="25"/>
       <c r="K3" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L3" s="15" t="s">
         <v>156</v>
@@ -6505,7 +6519,7 @@
         <v>70</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>51</v>
@@ -6521,7 +6535,7 @@
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>157</v>
@@ -6551,7 +6565,7 @@
         <v>88</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>15</v>
@@ -6567,7 +6581,7 @@
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>158</v>
@@ -6597,7 +6611,7 @@
         <v>88</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>15</v>
@@ -6613,7 +6627,7 @@
       </c>
       <c r="J6" s="25"/>
       <c r="K6" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L6" s="15" t="s">
         <v>159</v>
@@ -6643,7 +6657,7 @@
         <v>88</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>51</v>
@@ -6659,7 +6673,7 @@
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>160</v>
@@ -6689,7 +6703,7 @@
         <v>111</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>15</v>
@@ -6705,7 +6719,7 @@
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>102</v>
@@ -6735,7 +6749,7 @@
         <v>111</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>15</v>
@@ -6751,7 +6765,7 @@
       </c>
       <c r="J9" s="25"/>
       <c r="K9" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>161</v>
@@ -6781,7 +6795,7 @@
         <v>111</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>51</v>
@@ -6797,7 +6811,7 @@
       </c>
       <c r="J10" s="25"/>
       <c r="K10" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>162</v>
@@ -6829,7 +6843,7 @@
         <v>112</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>15</v>
@@ -6845,7 +6859,7 @@
       </c>
       <c r="J11" s="25"/>
       <c r="K11" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L11" s="15" t="s">
         <v>163</v>
@@ -6875,7 +6889,7 @@
         <v>112</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>15</v>
@@ -6891,7 +6905,7 @@
       </c>
       <c r="J12" s="25"/>
       <c r="K12" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L12" s="15" t="s">
         <v>164</v>
@@ -6921,7 +6935,7 @@
         <v>112</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>51</v>
@@ -6937,7 +6951,7 @@
       </c>
       <c r="J13" s="25"/>
       <c r="K13" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L13" s="15" t="s">
         <v>102</v>
@@ -6963,19 +6977,19 @@
         <v>66</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>47</v>
@@ -6985,7 +6999,7 @@
       </c>
       <c r="J14" s="25"/>
       <c r="K14" s="39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="L14" s="15" t="s">
         <v>165</v>
@@ -7067,7 +7081,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="60">
@@ -7078,7 +7092,7 @@
         <v>66</v>
       </c>
       <c r="C2" s="85" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D2" s="86" t="s">
         <v>256</v>
@@ -7096,10 +7110,10 @@
         <v>47</v>
       </c>
       <c r="I2" s="87" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J2" s="86" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="K2" s="84">
         <v>0</v>
@@ -7157,25 +7171,25 @@
         <v>16</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>690</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>691</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="44" t="s">
+        <v>605</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>692</v>
       </c>
-      <c r="I1" s="44" t="s">
-        <v>606</v>
-      </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="44" t="s">
         <v>693</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="L1" s="44" t="s">
         <v>694</v>
-      </c>
-      <c r="L1" s="44" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -7186,10 +7200,10 @@
         <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E2" s="39" t="s">
         <v>257</v>
@@ -7216,10 +7230,10 @@
         <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>258</v>
@@ -7234,7 +7248,7 @@
         <v>12345678</v>
       </c>
       <c r="I3" s="63" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="63"/>
@@ -7248,10 +7262,10 @@
         <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E4" s="39" t="s">
         <v>259</v>
@@ -7264,10 +7278,10 @@
         <v>12345678</v>
       </c>
       <c r="I4" s="63" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J4" s="63" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="K4" s="63"/>
       <c r="L4" s="47"/>
@@ -7280,10 +7294,10 @@
         <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>257</v>
@@ -7298,10 +7312,10 @@
         <v>12345678</v>
       </c>
       <c r="I5" s="63" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J5" s="63" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="K5" s="63"/>
       <c r="L5" s="47"/>
@@ -7314,10 +7328,10 @@
         <v>66</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E6" s="39" t="s">
         <v>258</v>
@@ -7330,11 +7344,11 @@
         <v>12345678</v>
       </c>
       <c r="I6" s="63" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J6" s="63"/>
       <c r="K6" s="63" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="L6" s="47"/>
     </row>
@@ -7346,10 +7360,10 @@
         <v>66</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E7" s="39" t="s">
         <v>259</v>
@@ -7364,11 +7378,11 @@
         <v>12345678</v>
       </c>
       <c r="I7" s="63" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J7" s="63"/>
       <c r="K7" s="63" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="L7" s="47"/>
     </row>
@@ -7380,10 +7394,10 @@
         <v>66</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>257</v>
@@ -7396,12 +7410,12 @@
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="63" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J8" s="63"/>
       <c r="K8" s="63"/>
       <c r="L8" s="63" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
@@ -7412,10 +7426,10 @@
         <v>66</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E9" s="39" t="s">
         <v>258</v>
@@ -7430,12 +7444,12 @@
         <v>123</v>
       </c>
       <c r="I9" s="63" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J9" s="63"/>
       <c r="K9" s="63"/>
       <c r="L9" s="63" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
@@ -7446,10 +7460,10 @@
         <v>66</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E10" s="39" t="s">
         <v>259</v>
@@ -7464,14 +7478,14 @@
         <v>123</v>
       </c>
       <c r="I10" s="63" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J10" s="63"/>
       <c r="K10" s="63" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="L10" s="63" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45">
@@ -7482,10 +7496,10 @@
         <v>66</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E11" s="39" t="s">
         <v>257</v>
@@ -7500,12 +7514,12 @@
         <v>123456798</v>
       </c>
       <c r="I11" s="63" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J11" s="63"/>
       <c r="K11" s="63"/>
       <c r="L11" s="63" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -8148,10 +8162,10 @@
         <v>4</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="G27" s="39" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -8171,10 +8185,10 @@
         <v>4</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G28" s="39" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -8197,7 +8211,7 @@
         <v>107</v>
       </c>
       <c r="G29" s="90" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -8220,7 +8234,7 @@
         <v>107</v>
       </c>
       <c r="G30" s="40" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -8243,7 +8257,7 @@
         <v>107</v>
       </c>
       <c r="G31" s="40" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -8266,7 +8280,7 @@
         <v>107</v>
       </c>
       <c r="G32" s="40" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -8289,7 +8303,7 @@
         <v>107</v>
       </c>
       <c r="G33" s="40" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -8312,7 +8326,7 @@
         <v>107</v>
       </c>
       <c r="G34" s="40" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -8335,7 +8349,7 @@
         <v>107</v>
       </c>
       <c r="G35" s="40" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -8358,7 +8372,7 @@
         <v>107</v>
       </c>
       <c r="G36" s="40" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -8381,7 +8395,7 @@
         <v>107</v>
       </c>
       <c r="G37" s="40" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -8404,7 +8418,7 @@
         <v>107</v>
       </c>
       <c r="G38" s="40" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -8427,7 +8441,7 @@
         <v>107</v>
       </c>
       <c r="G39" s="40" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -8450,7 +8464,7 @@
         <v>107</v>
       </c>
       <c r="G40" s="40" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -8473,7 +8487,7 @@
         <v>107</v>
       </c>
       <c r="G41" s="40" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -8496,7 +8510,7 @@
         <v>107</v>
       </c>
       <c r="G42" s="40" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -8519,7 +8533,7 @@
         <v>107</v>
       </c>
       <c r="G43" s="40" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -8542,7 +8556,7 @@
         <v>107</v>
       </c>
       <c r="G44" s="40" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -8565,7 +8579,7 @@
         <v>107</v>
       </c>
       <c r="G45" s="40" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -8588,7 +8602,7 @@
         <v>107</v>
       </c>
       <c r="G46" s="40" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -8611,7 +8625,7 @@
         <v>107</v>
       </c>
       <c r="G47" s="40" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -8634,7 +8648,7 @@
         <v>107</v>
       </c>
       <c r="G48" s="40" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -8657,7 +8671,7 @@
         <v>107</v>
       </c>
       <c r="G49" s="40" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -8680,7 +8694,7 @@
         <v>107</v>
       </c>
       <c r="G50" s="40" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -8703,7 +8717,7 @@
         <v>107</v>
       </c>
       <c r="G51" s="40" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -8726,7 +8740,7 @@
         <v>107</v>
       </c>
       <c r="G52" s="40" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -8749,7 +8763,7 @@
         <v>107</v>
       </c>
       <c r="G53" s="40" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -8772,7 +8786,7 @@
         <v>107</v>
       </c>
       <c r="G54" s="40" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -8795,7 +8809,7 @@
         <v>107</v>
       </c>
       <c r="G55" s="40" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -8818,7 +8832,7 @@
         <v>107</v>
       </c>
       <c r="G56" s="40" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -8841,7 +8855,7 @@
         <v>107</v>
       </c>
       <c r="G57" s="40" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -8864,7 +8878,7 @@
         <v>107</v>
       </c>
       <c r="G58" s="40" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -8887,7 +8901,7 @@
         <v>107</v>
       </c>
       <c r="G59" s="40" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -8910,7 +8924,7 @@
         <v>107</v>
       </c>
       <c r="G60" s="40" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -8933,7 +8947,7 @@
         <v>107</v>
       </c>
       <c r="G61" s="40" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -8956,7 +8970,7 @@
         <v>107</v>
       </c>
       <c r="G62" s="40" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -8979,7 +8993,7 @@
         <v>107</v>
       </c>
       <c r="G63" s="40" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -9002,7 +9016,7 @@
         <v>107</v>
       </c>
       <c r="G64" s="40" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -9025,7 +9039,7 @@
         <v>107</v>
       </c>
       <c r="G65" s="40" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
   </sheetData>
@@ -9095,7 +9109,7 @@
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A2" s="20" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>66</v>
@@ -9123,12 +9137,12 @@
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="13" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A3" s="20" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>66</v>
@@ -9156,12 +9170,12 @@
       </c>
       <c r="J3" s="25"/>
       <c r="K3" s="40" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A4" s="20" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>66</v>
@@ -9189,12 +9203,12 @@
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="40" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A5" s="20" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>66</v>
@@ -9222,12 +9236,12 @@
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="40" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A6" s="20" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>66</v>
@@ -9255,12 +9269,12 @@
       </c>
       <c r="J6" s="25"/>
       <c r="K6" s="40" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A7" s="20" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="23" t="s">
@@ -9286,12 +9300,12 @@
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="40" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A8" s="20" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="23" t="s">
@@ -9317,12 +9331,12 @@
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="40" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A9" s="20" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="23" t="s">
@@ -9348,12 +9362,12 @@
       </c>
       <c r="J9" s="25"/>
       <c r="K9" s="40" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A10" s="20" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="23" t="s">
@@ -9379,12 +9393,12 @@
       </c>
       <c r="J10" s="25"/>
       <c r="K10" s="40" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A11" s="20" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="23" t="s">
@@ -9410,12 +9424,12 @@
       </c>
       <c r="J11" s="25"/>
       <c r="K11" s="40" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="60">
       <c r="A12" s="20" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="23" t="s">
@@ -9441,12 +9455,12 @@
       </c>
       <c r="J12" s="25"/>
       <c r="K12" s="40" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60">
       <c r="A13" s="20" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="23" t="s">
@@ -9472,12 +9486,12 @@
       </c>
       <c r="J13" s="25"/>
       <c r="K13" s="40" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="60">
       <c r="A14" s="20" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="23" t="s">
@@ -9506,7 +9520,7 @@
     </row>
     <row r="15" spans="1:11" ht="60">
       <c r="A15" s="20" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="23" t="s">
@@ -9535,7 +9549,7 @@
     </row>
     <row r="16" spans="1:11" ht="60">
       <c r="A16" s="20" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="23" t="s">
@@ -9564,7 +9578,7 @@
     </row>
     <row r="17" spans="1:11" ht="60">
       <c r="A17" s="20" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="23" t="s">
@@ -9593,7 +9607,7 @@
     </row>
     <row r="18" spans="1:11" ht="60">
       <c r="A18" s="20" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="23" t="s">
@@ -9622,7 +9636,7 @@
     </row>
     <row r="19" spans="1:11" ht="60">
       <c r="A19" s="20" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="23" t="s">
@@ -9651,7 +9665,7 @@
     </row>
     <row r="20" spans="1:11" ht="60">
       <c r="A20" s="20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="23" t="s">
@@ -9677,12 +9691,12 @@
       </c>
       <c r="J20" s="25"/>
       <c r="K20" s="40" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="60">
       <c r="A21" s="20" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="23" t="s">
@@ -9708,12 +9722,12 @@
       </c>
       <c r="J21" s="25"/>
       <c r="K21" s="40" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="60">
       <c r="A22" s="20" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="23" t="s">
@@ -9739,12 +9753,12 @@
       </c>
       <c r="J22" s="25"/>
       <c r="K22" s="40" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60">
       <c r="A23" s="20" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="23" t="s">
@@ -9770,12 +9784,12 @@
       </c>
       <c r="J23" s="25"/>
       <c r="K23" s="40" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60">
       <c r="A24" s="20" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="23" t="s">
@@ -9801,12 +9815,12 @@
       </c>
       <c r="J24" s="25"/>
       <c r="K24" s="40" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60">
       <c r="A25" s="20" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="23" t="s">
@@ -9832,12 +9846,12 @@
       </c>
       <c r="J25" s="25"/>
       <c r="K25" s="40" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60">
       <c r="A26" s="20" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="23" t="s">
@@ -9863,12 +9877,12 @@
       </c>
       <c r="J26" s="25"/>
       <c r="K26" s="40" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60">
       <c r="A27" s="20" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="23" t="s">
@@ -9894,12 +9908,12 @@
       </c>
       <c r="J27" s="25"/>
       <c r="K27" s="40" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60">
       <c r="A28" s="20" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="23" t="s">
@@ -9925,12 +9939,12 @@
       </c>
       <c r="J28" s="25"/>
       <c r="K28" s="40" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60">
       <c r="A29" s="20" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B29" s="20"/>
       <c r="C29" s="23" t="s">
@@ -9956,12 +9970,12 @@
       </c>
       <c r="J29" s="25"/>
       <c r="K29" s="40" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60">
       <c r="A30" s="20" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B30" s="20"/>
       <c r="C30" s="23" t="s">
@@ -9987,12 +10001,12 @@
       </c>
       <c r="J30" s="25"/>
       <c r="K30" s="40" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60">
       <c r="A31" s="20" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="23" t="s">
@@ -10018,12 +10032,12 @@
       </c>
       <c r="J31" s="25"/>
       <c r="K31" s="40" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="60">
       <c r="A32" s="20" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B32" s="20"/>
       <c r="C32" s="23" t="s">
@@ -10052,7 +10066,7 @@
     </row>
     <row r="33" spans="1:11" ht="60">
       <c r="A33" s="20" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="23" t="s">
@@ -10081,7 +10095,7 @@
     </row>
     <row r="34" spans="1:11" ht="60">
       <c r="A34" s="20" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="23" t="s">
@@ -10110,7 +10124,7 @@
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" s="20" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="23" t="s">
@@ -10139,7 +10153,7 @@
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" s="20" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="23" t="s">
@@ -10168,7 +10182,7 @@
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" s="20" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="23" t="s">
@@ -10197,7 +10211,7 @@
     </row>
     <row r="38" spans="1:11" ht="60">
       <c r="A38" s="20" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="23" t="s">
@@ -10226,7 +10240,7 @@
     </row>
     <row r="39" spans="1:11" ht="60">
       <c r="A39" s="20" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="23" t="s">
@@ -10236,7 +10250,7 @@
         <v>105</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F39" s="23" t="s">
         <v>51</v>
@@ -10286,7 +10300,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>82</v>
@@ -10304,19 +10318,19 @@
         <v>13</v>
       </c>
       <c r="H1" s="70" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I1" s="70" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="J1" s="70" t="s">
         <v>18</v>
       </c>
       <c r="K1" s="70" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="L1" s="70" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="60">
@@ -10324,10 +10338,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D2" s="79" t="s">
         <v>75</v>
@@ -10352,10 +10366,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D3" s="79" t="s">
         <v>79</v>
@@ -10380,10 +10394,10 @@
         <v>78</v>
       </c>
       <c r="B4" s="31" t="s">
+        <v>736</v>
+      </c>
+      <c r="C4" s="32" t="s">
         <v>737</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>738</v>
       </c>
       <c r="D4" s="79" t="s">
         <v>193</v>
@@ -10404,10 +10418,10 @@
         <v>170</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D5" s="79" t="s">
         <v>171</v>
@@ -10428,10 +10442,10 @@
         <v>200</v>
       </c>
       <c r="B6" s="31" t="s">
+        <v>736</v>
+      </c>
+      <c r="C6" s="32" t="s">
         <v>737</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>738</v>
       </c>
       <c r="D6" s="80" t="s">
         <v>193</v>
@@ -10449,16 +10463,16 @@
     </row>
     <row r="7" spans="1:12" ht="75">
       <c r="A7" s="31" t="s">
+        <v>712</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>802</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>728</v>
+      </c>
+      <c r="D7" s="79" t="s">
         <v>713</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>803</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>729</v>
-      </c>
-      <c r="D7" s="79" t="s">
-        <v>714</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
@@ -10466,33 +10480,33 @@
         <v>201</v>
       </c>
       <c r="H7" s="28" t="s">
+        <v>724</v>
+      </c>
+      <c r="I7" s="25" t="s">
         <v>725</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="J7" s="28" t="s">
         <v>726</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>727</v>
       </c>
       <c r="K7" s="25" t="s">
         <v>168</v>
       </c>
       <c r="L7" s="25" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="75">
       <c r="A8" s="31" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
@@ -10501,7 +10515,7 @@
       </c>
       <c r="H8" s="28"/>
       <c r="I8" s="25" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="J8" s="28"/>
       <c r="K8" s="25"/>
@@ -10623,10 +10637,10 @@
     </row>
     <row r="7" spans="1:5" ht="75">
       <c r="A7" s="19" t="s">
+        <v>712</v>
+      </c>
+      <c r="B7" s="43" t="s">
         <v>713</v>
-      </c>
-      <c r="B7" s="43" t="s">
-        <v>714</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -10926,7 +10940,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="14" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>3</v>
@@ -10938,13 +10952,13 @@
         <v>83</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>38</v>
@@ -15114,13 +15128,13 @@
         <v>17</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="44" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="105">
@@ -15131,13 +15145,13 @@
         <v>66</v>
       </c>
       <c r="C2" s="72" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D2" s="72" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E2" s="72" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F2" s="73"/>
       <c r="G2" s="74"/>
@@ -15148,13 +15162,13 @@
       </c>
       <c r="B3" s="46"/>
       <c r="C3" s="72" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D3" s="72" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F3" s="73"/>
       <c r="G3" s="75"/>
@@ -15165,13 +15179,13 @@
       </c>
       <c r="B4" s="46"/>
       <c r="C4" s="72" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D4" s="72" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E4" s="72" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F4" s="73"/>
       <c r="G4" s="75"/>
@@ -15182,13 +15196,13 @@
       </c>
       <c r="B5" s="46"/>
       <c r="C5" s="72" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D5" s="72" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E5" s="72" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F5" s="73"/>
       <c r="G5" s="75"/>
@@ -15939,32 +15953,31 @@
   <sheetPr codeName="Sheet5">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.5703125" style="52" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.7109375" style="52" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="20.7109375" style="52" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="4" collapsed="1"/>
-    <col min="13" max="13" width="15.140625" style="52" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.85546875" style="52" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.5703125" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.7109375" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="20.7109375" style="52" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="4" collapsed="1"/>
+    <col min="12" max="12" width="15.140625" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.85546875" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="19.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1">
+    <row r="1" spans="1:18" s="6" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>93</v>
       </c>
@@ -15974,58 +15987,55 @@
       <c r="C1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>574</v>
       </c>
+      <c r="E1" s="10" t="s">
+        <v>575</v>
+      </c>
       <c r="F1" s="10" t="s">
-        <v>575</v>
-      </c>
-      <c r="G1" s="10" t="s">
         <v>576</v>
       </c>
+      <c r="G1" s="44" t="s">
+        <v>577</v>
+      </c>
       <c r="H1" s="44" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>579</v>
-      </c>
-      <c r="K1" s="44" t="s">
         <v>580</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>581</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="L1" s="45" t="s">
         <v>582</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="M1" s="44" t="s">
         <v>583</v>
       </c>
+      <c r="N1" s="10" t="s">
+        <v>584</v>
+      </c>
       <c r="O1" s="10" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>587</v>
-      </c>
-      <c r="S1" s="10" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="4" customFormat="1">
+    <row r="2" spans="1:18" s="4" customFormat="1">
       <c r="A2" s="46" t="s">
-        <v>94</v>
+        <v>944</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>66</v>
@@ -16033,7 +16043,7 @@
       <c r="C2" s="7" t="s">
         <v>589</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="7" t="s">
         <v>590</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -16042,29 +16052,29 @@
       <c r="F2" s="7" t="s">
         <v>592</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="47">
+        <v>300389093</v>
+      </c>
+      <c r="H2" s="47">
+        <v>3003890930</v>
+      </c>
+      <c r="I2" s="48">
+        <v>1</v>
+      </c>
+      <c r="J2" s="48">
+        <v>3</v>
+      </c>
+      <c r="K2" s="49" t="s">
         <v>593</v>
       </c>
-      <c r="H2" s="47">
-        <v>300389093</v>
-      </c>
-      <c r="I2" s="47">
-        <v>3003890930</v>
-      </c>
-      <c r="J2" s="48">
+      <c r="L2" s="50">
+        <v>3</v>
+      </c>
+      <c r="M2" s="51">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="K2" s="48">
-        <v>3</v>
-      </c>
-      <c r="L2" s="49" t="s">
-        <v>594</v>
-      </c>
-      <c r="M2" s="50">
-        <v>3</v>
-      </c>
-      <c r="N2" s="51">
-        <v>0</v>
       </c>
       <c r="O2" s="7" t="b">
         <v>1</v>
@@ -16073,25 +16083,24 @@
         <v>1</v>
       </c>
       <c r="Q2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="R2" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="46"/>
+        <v>945</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>66</v>
+      </c>
       <c r="C3" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>595</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>590</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>596</v>
@@ -16099,29 +16108,29 @@
       <c r="F3" s="7" t="s">
         <v>597</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>598</v>
+      <c r="G3" s="47">
+        <v>300389094</v>
       </c>
       <c r="H3" s="47">
-        <v>300389094</v>
+        <v>3003890940</v>
       </c>
       <c r="I3" s="47">
-        <v>3003890940</v>
+        <v>1</v>
       </c>
       <c r="J3" s="47">
         <v>1</v>
       </c>
-      <c r="K3" s="47">
+      <c r="K3" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="L3" s="50">
+        <v>2</v>
+      </c>
+      <c r="M3" s="51">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7" t="b">
         <v>1</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>599</v>
-      </c>
-      <c r="M3" s="50">
-        <v>2</v>
-      </c>
-      <c r="N3" s="51">
-        <v>0</v>
       </c>
       <c r="O3" s="7" t="b">
         <v>1</v>
@@ -16130,147 +16139,142 @@
         <v>1</v>
       </c>
       <c r="Q3" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="S3" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="46"/>
+        <v>946</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>66</v>
+      </c>
       <c r="C4" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="E4" s="7" t="s">
         <v>590</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>601</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>591</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>593</v>
+        <v>592</v>
+      </c>
+      <c r="G4" s="47">
+        <v>300389095</v>
       </c>
       <c r="H4" s="47">
-        <v>300389095</v>
+        <v>3003890950</v>
       </c>
       <c r="I4" s="47">
-        <v>3003890950</v>
+        <v>1</v>
       </c>
       <c r="J4" s="47">
         <v>1</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="L4" s="50">
         <v>1</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="M4" s="50">
+      <c r="M4" s="51">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="N4" s="51">
+      <c r="O4" s="7" t="b">
         <v>0</v>
-      </c>
-      <c r="O4" s="7" t="b">
-        <v>1</v>
       </c>
       <c r="P4" s="7" t="b">
         <v>0</v>
       </c>
       <c r="Q4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="R4" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="S4" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="46"/>
+        <v>947</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>66</v>
+      </c>
       <c r="C5" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>603</v>
       </c>
-      <c r="D5" s="39" t="s">
-        <v>590</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>601</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>593</v>
+        <v>592</v>
+      </c>
+      <c r="G5" s="47">
+        <v>300389095</v>
       </c>
       <c r="H5" s="47">
-        <v>300389095</v>
+        <v>3003890960</v>
       </c>
       <c r="I5" s="47">
-        <v>3003890960</v>
+        <v>2</v>
       </c>
       <c r="J5" s="47">
         <v>2</v>
       </c>
-      <c r="K5" s="47">
-        <v>2</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="50">
+      <c r="L5" s="50">
         <v>0</v>
       </c>
-      <c r="N5" s="51">
+      <c r="M5" s="51">
         <v>0</v>
       </c>
+      <c r="N5" s="7" t="b">
+        <v>1</v>
+      </c>
       <c r="O5" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="7" t="b">
         <v>0</v>
       </c>
       <c r="Q5" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="S5" s="7" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" display="ibatta@dbi.com"/>
-    <hyperlink ref="N3" r:id="rId2" display="ibatta@dbi.com"/>
-    <hyperlink ref="N4" r:id="rId3" display="ibatta@dbi.com"/>
-    <hyperlink ref="N5" r:id="rId4" display="ibatta@dbi.com"/>
-    <hyperlink ref="O2" r:id="rId5" display="ibatta@dbi.com"/>
-    <hyperlink ref="R2" r:id="rId6" display="ibatta@dbi.com"/>
-    <hyperlink ref="O3:O5" r:id="rId7" display="ibatta@dbi.com"/>
-    <hyperlink ref="P2" r:id="rId8" display="ibatta@dbi.com"/>
-    <hyperlink ref="O3" r:id="rId9" display="ibatta@dbi.com"/>
-    <hyperlink ref="Q2" r:id="rId10" display="ibatta@dbi.com"/>
-    <hyperlink ref="P3" r:id="rId11" display="ibatta@dbi.com"/>
-    <hyperlink ref="Q3" r:id="rId12" display="ibatta@dbi.com"/>
-    <hyperlink ref="R3" r:id="rId13" display="ibatta@dbi.com"/>
-    <hyperlink ref="S2" r:id="rId14" display="ibatta@dbi.com"/>
-    <hyperlink ref="S3" r:id="rId15" display="ibatta@dbi.com"/>
-    <hyperlink ref="S4:S5" r:id="rId16" display="ibatta@dbi.com"/>
+    <hyperlink ref="M2" r:id="rId1" display="ibatta@dbi.com"/>
+    <hyperlink ref="M3" r:id="rId2" display="ibatta@dbi.com"/>
+    <hyperlink ref="M4" r:id="rId3" display="ibatta@dbi.com"/>
+    <hyperlink ref="M5" r:id="rId4" display="ibatta@dbi.com"/>
+    <hyperlink ref="N2" r:id="rId5" display="ibatta@dbi.com"/>
+    <hyperlink ref="Q2" r:id="rId6" display="ibatta@dbi.com"/>
+    <hyperlink ref="N3:N5" r:id="rId7" display="ibatta@dbi.com"/>
+    <hyperlink ref="O2" r:id="rId8" display="ibatta@dbi.com"/>
+    <hyperlink ref="N3" r:id="rId9" display="ibatta@dbi.com"/>
+    <hyperlink ref="P2" r:id="rId10" display="ibatta@dbi.com"/>
+    <hyperlink ref="O3" r:id="rId11" display="ibatta@dbi.com"/>
+    <hyperlink ref="P3" r:id="rId12" display="ibatta@dbi.com"/>
+    <hyperlink ref="Q3" r:id="rId13" display="ibatta@dbi.com"/>
+    <hyperlink ref="R2" r:id="rId14" display="ibatta@dbi.com"/>
+    <hyperlink ref="R3" r:id="rId15" display="ibatta@dbi.com"/>
+    <hyperlink ref="R4:R5" r:id="rId16" display="ibatta@dbi.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId17"/>
@@ -16319,19 +16323,19 @@
         <v>108</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G1" s="22" t="s">
         <v>41</v>
       </c>
       <c r="H1" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>606</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="22" t="s">
         <v>607</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -16342,10 +16346,10 @@
         <v>66</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E2" s="40" t="s">
         <v>260</v>
@@ -16368,19 +16372,19 @@
         <v>66</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>261</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H3" s="58"/>
       <c r="I3" s="58"/>
@@ -16394,22 +16398,22 @@
         <v>66</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E4" s="40" t="s">
         <v>262</v>
       </c>
       <c r="F4" s="28" t="s">
+        <v>647</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="H4" s="76" t="s">
         <v>648</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>655</v>
-      </c>
-      <c r="H4" s="76" t="s">
-        <v>649</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="58"/>
@@ -16422,20 +16426,20 @@
         <v>66</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E5" s="40" t="s">
         <v>263</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H5" s="76" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I5" s="58" t="s">
         <v>1</v>
@@ -16450,20 +16454,20 @@
         <v>66</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E6" s="40" t="s">
         <v>264</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G6" s="28"/>
       <c r="H6" s="76" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I6" s="58"/>
       <c r="J6" s="58" t="s">
@@ -16478,10 +16482,10 @@
         <v>66</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E7" s="40" t="s">
         <v>265</v>
@@ -16489,7 +16493,7 @@
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="76" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I7" s="58" t="s">
         <v>1</v>
@@ -16506,22 +16510,22 @@
         <v>66</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E8" s="40" t="s">
         <v>266</v>
       </c>
       <c r="F8" s="28" t="s">
+        <v>647</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="H8" s="76" t="s">
         <v>648</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>655</v>
-      </c>
-      <c r="H8" s="76" t="s">
-        <v>649</v>
       </c>
       <c r="I8" s="58"/>
       <c r="J8" s="58"/>
@@ -16571,13 +16575,13 @@
         <v>8</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>616</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45">
@@ -16588,19 +16592,19 @@
         <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D2" s="69" t="s">
         <v>256</v>
       </c>
       <c r="E2" s="66" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>620</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>621</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -16614,19 +16618,19 @@
         <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D3" s="69" t="s">
         <v>257</v>
       </c>
       <c r="E3" s="66" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
@@ -16640,13 +16644,13 @@
         <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="D4" s="83" t="s">
         <v>709</v>
       </c>
-      <c r="D4" s="83" t="s">
-        <v>710</v>
-      </c>
       <c r="E4" s="66" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -16695,7 +16699,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="60" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -16706,13 +16710,13 @@
         <v>66</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>627</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>629</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -16723,13 +16727,13 @@
         <v>66</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>632</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="105">
@@ -16740,13 +16744,13 @@
         <v>66</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>634</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="62" t="s">
         <v>635</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -16757,13 +16761,13 @@
         <v>66</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>638</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -16774,13 +16778,13 @@
         <v>66</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>640</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>641</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
@@ -16791,13 +16795,13 @@
         <v>66</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>642</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="62" t="s">
         <v>643</v>
-      </c>
-      <c r="E7" s="62" t="s">
-        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -16857,7 +16861,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="56" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B2" s="56" t="s">
         <v>66</v>
@@ -16874,7 +16878,7 @@
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="56" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B3" s="56" t="s">
         <v>66</v>
@@ -16886,12 +16890,12 @@
         <v>257</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
       <c r="A4" s="56" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B4" s="56" t="s">
         <v>66</v>
@@ -16903,12 +16907,12 @@
         <v>258</v>
       </c>
       <c r="E4" s="56" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
       <c r="A5" s="56" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B5" s="56" t="s">
         <v>66</v>
@@ -16920,12 +16924,12 @@
         <v>259</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="56" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B6" s="56" t="s">
         <v>66</v>

</xml_diff>